<commit_message>
EST-1134: fleshes out IncomingCharge with fixture and integtest
</commit_message>
<xml_diff>
--- a/estatioapp/module/capex/dom/src/main/java/org/estatio/capex/fixture/charge/CapexChargeHierarchy.xlsx
+++ b/estatioapp/module/capex/dom/src/main/java/org/estatio/capex/fixture/charge/CapexChargeHierarchy.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\estatio\estatio\estatioapp\module\capex\dom\src\main\java\org\estatio\capex\fixture\charge\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
-  <si>
-    <t>Charges</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
   <si>
     <t>PROJECT MANAGEMENT</t>
   </si>
@@ -39,9 +36,6 @@
     <t>ARCHITECT / GEOMETRICIAN FEES</t>
   </si>
   <si>
-    <t>LEGAL FEES</t>
-  </si>
-  <si>
     <t>MARKETING</t>
   </si>
   <si>
@@ -57,10 +51,22 @@
     <t>OTHER</t>
   </si>
   <si>
-    <t>ChargeParent</t>
-  </si>
-  <si>
     <t>FRANCE</t>
+  </si>
+  <si>
+    <t>LEGAL / BAILIFF FEES</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>AtPath</t>
+  </si>
+  <si>
+    <t>/FRA</t>
   </si>
 </sst>
 </file>
@@ -124,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -135,6 +141,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,7 +460,7 @@
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -463,12 +471,14 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="D1" s="3"/>
       <c r="E1" s="2"/>
       <c r="F1" s="3"/>
@@ -495,10 +505,12 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
+      <c r="C2" s="11" t="s">
+        <v>15</v>
+      </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
       <c r="F2" s="3"/>
@@ -525,124 +537,146 @@
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="D6" s="5"/>
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="D7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">

</xml_diff>

<commit_message>
EST-1338: charge INSURANCE added to charge list for capex
</commit_message>
<xml_diff>
--- a/estatioapp/module/capex/dom/src/main/java/org/estatio/capex/fixture/charge/CapexChargeHierarchy.xlsx
+++ b/estatioapp/module/capex/dom/src/main/java/org/estatio/capex/fixture/charge/CapexChargeHierarchy.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\estatio\estatio\estatioapp\module\capex\dom\src\main\java\org\estatio\capex\fixture\charge\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27880" windowHeight="12800"/>
   </bookViews>
   <sheets>
     <sheet name="ChargeHierarchy" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
   <si>
     <t>PROJECT MANAGEMENT</t>
   </si>
@@ -67,13 +67,16 @@
   </si>
   <si>
     <t>/FRA</t>
+  </si>
+  <si>
+    <t>INSURANCE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -103,6 +106,18 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -127,8 +142,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -144,7 +161,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -203,7 +222,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -255,7 +274,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -449,7 +468,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -460,16 +479,16 @@
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="38.5703125" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" customWidth="1"/>
+    <col min="1" max="1" width="38.5" customWidth="1"/>
+    <col min="5" max="5" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" ht="14">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -503,7 +522,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" ht="14">
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
@@ -535,7 +554,7 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" ht="14">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -549,7 +568,7 @@
       <c r="E3" s="5"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" ht="14">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -563,7 +582,7 @@
       <c r="E4" s="5"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" ht="14">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -577,7 +596,7 @@
       <c r="E5" s="5"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" ht="14">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -590,7 +609,7 @@
       <c r="D6" s="5"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" ht="14">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -604,7 +623,7 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" ht="14">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
@@ -617,7 +636,7 @@
       <c r="D8" s="5"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" ht="14">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -630,7 +649,7 @@
       <c r="D9" s="5"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" ht="14">
       <c r="A10" s="7" t="s">
         <v>6</v>
       </c>
@@ -643,7 +662,7 @@
       <c r="D10" s="5"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" ht="14">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -655,7 +674,7 @@
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" ht="14">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
@@ -667,24 +686,37 @@
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" ht="14">
       <c r="A13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:26" ht="15" customHeight="1">
+      <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:26" ht="15" customHeight="1">
-      <c r="C14" s="5"/>
+      <c r="B14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="D14" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EST-1338: adds FURNITURES / DECORATION as charge for capex
</commit_message>
<xml_diff>
--- a/estatioapp/module/capex/dom/src/main/java/org/estatio/capex/fixture/charge/CapexChargeHierarchy.xlsx
+++ b/estatioapp/module/capex/dom/src/main/java/org/estatio/capex/fixture/charge/CapexChargeHierarchy.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="18">
   <si>
     <t>PROJECT MANAGEMENT</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>INSURANCE</t>
+  </si>
+  <si>
+    <t>FURNITURES / DECORATION</t>
   </si>
 </sst>
 </file>
@@ -142,8 +145,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -161,9 +168,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -468,7 +479,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -476,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z14"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -700,15 +711,26 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:26" ht="15" customHeight="1">
+      <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="5"/>
+      <c r="B15" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>